<commit_message>
cca terricole + histogramme pollution metaux lourds
</commit_message>
<xml_diff>
--- a/RAW2/IUCN_bee_sp-each-site(genus-and-familly).xlsx
+++ b/RAW2/IUCN_bee_sp-each-site(genus-and-familly).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - UMONS\UMONS\MA2\MEMOIRE\Statistique\R\STAT-MEMOIRE\RAW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniumonsac-my.sharepoint.com/personal/151201_umons_ac_be/Documents/UMONS/MA2/MEMOIRE/Statistique/R/STAT-MEMOIRE/RAW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577B2383-E095-4144-B467-A6DB3560C91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{577B2383-E095-4144-B467-A6DB3560C91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90977C25-D718-4046-B2F8-0C88A22CE7AC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3015" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cible" sheetId="2" r:id="rId1"/>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:F461"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>